<commit_message>
Remove empty line in NoticeBoard component
</commit_message>
<xml_diff>
--- a/public/tentative_schdule.xlsx
+++ b/public/tentative_schdule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OS\Desktop\DHE Ka Kaam\rase\rase-co-in\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OS\Desktop\DHE Ka Kaam\DHE\dhe-org-in\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95ACD2D2-5EB0-44BA-A975-EB4D81D2755B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0E6EBB-B7E4-4927-88AE-C8E1E24D54CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule-SM2024" sheetId="1" r:id="rId1"/>
@@ -429,9 +429,6 @@
     <xf numFmtId="20" fontId="7" fillId="3" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,6 +437,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -757,7 +757,7 @@
   <dimension ref="B1:C141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,26 +767,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="16"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="2:3" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="16"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" spans="2:3" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="16"/>
     </row>
     <row r="4" spans="2:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
     </row>
     <row r="5" spans="2:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -959,13 +959,13 @@
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="19"/>
+      <c r="B33" s="18"/>
       <c r="C33" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="19"/>
+      <c r="B34" s="18"/>
       <c r="C34" s="7" t="s">
         <v>14</v>
       </c>
@@ -1059,14 +1059,14 @@
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="2:3" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="17"/>
+      <c r="C50" s="16"/>
     </row>
     <row r="51" spans="2:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
@@ -1221,13 +1221,13 @@
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B77" s="19"/>
+      <c r="B77" s="18"/>
       <c r="C77" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B78" s="19"/>
+      <c r="B78" s="18"/>
       <c r="C78" s="7" t="s">
         <v>14</v>
       </c>
@@ -1339,14 +1339,14 @@
       <c r="C96" s="1"/>
     </row>
     <row r="97" spans="2:3" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C97" s="17"/>
+      <c r="C97" s="16"/>
     </row>
     <row r="98" spans="2:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B98" s="18"/>
-      <c r="C98" s="18"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="17"/>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B99" s="2" t="s">
@@ -1507,13 +1507,13 @@
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B125" s="19"/>
+      <c r="B125" s="18"/>
       <c r="C125" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B126" s="19"/>
+      <c r="B126" s="18"/>
       <c r="C126" s="7" t="s">
         <v>12</v>
       </c>
@@ -1610,17 +1610,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B125:B126"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B77:B78"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B77:B78"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="81" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>